<commit_message>
update ten file report co so
</commit_message>
<xml_diff>
--- a/Notion data/Chấm công HỆ THỐNG.xlsx
+++ b/Notion data/Chấm công HỆ THỐNG.xlsx
@@ -262,10 +262,10 @@
     <t>2024-07-02T18:08:00.000Z</t>
   </si>
   <si>
-    <t>2024-08-03T03:17:00.000Z</t>
-  </si>
-  <si>
-    <t>2024-08-03T03:18:00.000Z</t>
+    <t>2024-08-03T03:28:00.000Z</t>
+  </si>
+  <si>
+    <t>2024-08-03T03:29:00.000Z</t>
   </si>
   <si>
     <t>https://www.notion.so/11-3591e46ba1b0448ea0a6afcd443b310e</t>
@@ -3054,7 +3054,7 @@
         <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
collect data thuong phat
</commit_message>
<xml_diff>
--- a/Notion data/Chấm công HỆ THỐNG.xlsx
+++ b/Notion data/Chấm công HỆ THỐNG.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="171">
   <si>
     <t>object</t>
   </si>
@@ -262,10 +262,7 @@
     <t>2024-07-02T18:08:00.000Z</t>
   </si>
   <si>
-    <t>2024-08-03T03:28:00.000Z</t>
-  </si>
-  <si>
-    <t>2024-08-03T03:29:00.000Z</t>
+    <t>2024-08-03T03:54:00.000Z</t>
   </si>
   <si>
     <t>https://www.notion.so/11-3591e46ba1b0448ea0a6afcd443b310e</t>
@@ -1087,136 +1084,136 @@
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" t="s">
         <v>105</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" t="s">
         <v>106</v>
       </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>107</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>108</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>109</v>
       </c>
-      <c r="Q2" t="s">
-        <v>110</v>
-      </c>
       <c r="R2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>111</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
         <v>112</v>
       </c>
-      <c r="U2" t="s">
-        <v>111</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
         <v>113</v>
       </c>
-      <c r="X2" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>114</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>115</v>
       </c>
-      <c r="AB2" t="s">
-        <v>116</v>
-      </c>
       <c r="AC2" t="b">
         <v>0</v>
       </c>
       <c r="AD2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF2">
+        <v>2</v>
+      </c>
+      <c r="AG2" t="s">
         <v>137</v>
       </c>
-      <c r="AE2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF2">
-        <v>2</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI2">
+        <v>2</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>138</v>
       </c>
-      <c r="AH2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI2">
-        <v>2</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>139</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM2">
+        <v>2</v>
+      </c>
+      <c r="AN2" t="s">
         <v>140</v>
       </c>
-      <c r="AL2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM2">
-        <v>2</v>
-      </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2" t="s">
         <v>141</v>
       </c>
-      <c r="AO2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>142</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>143</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>144</v>
       </c>
-      <c r="AT2" t="s">
-        <v>145</v>
-      </c>
       <c r="AU2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV2" t="s">
         <v>148</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="s">
         <v>149</v>
       </c>
-      <c r="AW2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA2" t="s">
         <v>150</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>150</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:53">
@@ -1239,136 +1236,136 @@
         <v>0</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" t="s">
         <v>105</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
         <v>106</v>
       </c>
-      <c r="M3" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>107</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>108</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>109</v>
       </c>
-      <c r="Q3" t="s">
-        <v>110</v>
-      </c>
       <c r="R3" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3" t="s">
         <v>111</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" t="s">
         <v>112</v>
       </c>
-      <c r="U3" t="s">
-        <v>111</v>
-      </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3" t="s">
         <v>113</v>
       </c>
-      <c r="X3" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>114</v>
       </c>
-      <c r="AA3" t="s">
-        <v>115</v>
-      </c>
       <c r="AB3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AC3" t="b">
         <v>0</v>
       </c>
       <c r="AD3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF3">
+        <v>2</v>
+      </c>
+      <c r="AG3" t="s">
         <v>137</v>
       </c>
-      <c r="AE3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF3">
-        <v>2</v>
-      </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+      <c r="AJ3" t="s">
         <v>138</v>
       </c>
-      <c r="AH3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI3">
-        <v>2</v>
-      </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>139</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM3">
+        <v>2</v>
+      </c>
+      <c r="AN3" t="s">
         <v>140</v>
       </c>
-      <c r="AL3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM3">
-        <v>2</v>
-      </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>141</v>
       </c>
-      <c r="AO3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="s">
+      <c r="AR3" t="s">
         <v>142</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AS3" t="s">
         <v>143</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AT3" t="s">
         <v>144</v>
       </c>
-      <c r="AT3" t="s">
-        <v>145</v>
-      </c>
       <c r="AU3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV3" t="s">
         <v>148</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AW3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX3">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="s">
         <v>149</v>
       </c>
-      <c r="AW3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX3">
-        <v>0</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:53">
@@ -1391,136 +1388,136 @@
         <v>0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" t="s">
         <v>105</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" t="s">
         <v>106</v>
       </c>
-      <c r="M4" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>107</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>108</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>109</v>
       </c>
-      <c r="Q4" t="s">
-        <v>110</v>
-      </c>
       <c r="R4" t="s">
+        <v>110</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s">
         <v>111</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
+        <v>110</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4" t="s">
         <v>112</v>
       </c>
-      <c r="U4" t="s">
-        <v>111</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="s">
         <v>113</v>
       </c>
-      <c r="X4" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>114</v>
       </c>
-      <c r="AA4" t="s">
-        <v>115</v>
-      </c>
       <c r="AB4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AC4" t="b">
         <v>0</v>
       </c>
       <c r="AD4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF4">
+        <v>2</v>
+      </c>
+      <c r="AG4" t="s">
         <v>137</v>
       </c>
-      <c r="AE4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF4">
-        <v>2</v>
-      </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>138</v>
       </c>
-      <c r="AH4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI4">
-        <v>2</v>
-      </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>139</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AL4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM4">
+        <v>2</v>
+      </c>
+      <c r="AN4" t="s">
         <v>140</v>
       </c>
-      <c r="AL4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM4">
-        <v>2</v>
-      </c>
-      <c r="AN4" t="s">
+      <c r="AO4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="s">
         <v>141</v>
       </c>
-      <c r="AO4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AR4" t="s">
         <v>142</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AS4" t="s">
         <v>143</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AT4" t="s">
         <v>144</v>
       </c>
-      <c r="AT4" t="s">
-        <v>145</v>
-      </c>
       <c r="AU4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV4" t="s">
         <v>148</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="AW4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX4">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="s">
         <v>149</v>
       </c>
-      <c r="AW4" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX4">
-        <v>0</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:53">
@@ -1543,136 +1540,136 @@
         <v>0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" t="s">
         <v>105</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" t="s">
         <v>106</v>
       </c>
-      <c r="M5" t="s">
-        <v>105</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>107</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>108</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" t="s">
-        <v>110</v>
-      </c>
       <c r="R5" t="s">
+        <v>110</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s">
         <v>111</v>
       </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
+        <v>110</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5" t="s">
         <v>112</v>
       </c>
-      <c r="U5" t="s">
-        <v>111</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5" t="s">
         <v>113</v>
       </c>
-      <c r="X5" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>114</v>
       </c>
-      <c r="AA5" t="s">
-        <v>115</v>
-      </c>
       <c r="AB5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AC5" t="b">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF5">
+        <v>2</v>
+      </c>
+      <c r="AG5" t="s">
         <v>137</v>
       </c>
-      <c r="AE5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF5">
-        <v>2</v>
-      </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI5">
+        <v>2</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>138</v>
       </c>
-      <c r="AH5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI5">
-        <v>2</v>
-      </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>139</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM5">
+        <v>2</v>
+      </c>
+      <c r="AN5" t="s">
         <v>140</v>
       </c>
-      <c r="AL5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM5">
-        <v>2</v>
-      </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="s">
         <v>141</v>
       </c>
-      <c r="AO5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>142</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>143</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>144</v>
       </c>
-      <c r="AT5" t="s">
-        <v>145</v>
-      </c>
       <c r="AU5" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV5" t="s">
         <v>148</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX5">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="s">
         <v>149</v>
       </c>
-      <c r="AW5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX5">
-        <v>0</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:53">
@@ -1695,136 +1692,136 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" t="s">
         <v>105</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" t="s">
         <v>106</v>
       </c>
-      <c r="M6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>107</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>108</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>109</v>
       </c>
-      <c r="Q6" t="s">
-        <v>110</v>
-      </c>
       <c r="R6" t="s">
+        <v>110</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
         <v>111</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
+        <v>110</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
         <v>112</v>
       </c>
-      <c r="U6" t="s">
-        <v>111</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
         <v>113</v>
       </c>
-      <c r="X6" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>114</v>
       </c>
-      <c r="AA6" t="s">
-        <v>115</v>
-      </c>
       <c r="AB6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC6" t="b">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="s">
         <v>137</v>
       </c>
-      <c r="AE6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>138</v>
       </c>
-      <c r="AH6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI6">
-        <v>0</v>
-      </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>139</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6" t="s">
         <v>140</v>
       </c>
-      <c r="AL6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="s">
         <v>141</v>
       </c>
-      <c r="AO6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>142</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>143</v>
       </c>
-      <c r="AS6" t="s">
-        <v>144</v>
-      </c>
       <c r="AT6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV6" t="s">
         <v>148</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX6">
+        <v>0</v>
+      </c>
+      <c r="AY6" t="s">
         <v>149</v>
       </c>
-      <c r="AW6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX6">
-        <v>0</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:53">
@@ -1847,136 +1844,136 @@
         <v>0</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L7" t="s">
         <v>105</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>104</v>
+      </c>
+      <c r="N7" t="s">
         <v>106</v>
       </c>
-      <c r="M7" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>107</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>108</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>109</v>
       </c>
-      <c r="Q7" t="s">
-        <v>110</v>
-      </c>
       <c r="R7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
         <v>111</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
+        <v>110</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7" t="s">
         <v>112</v>
       </c>
-      <c r="U7" t="s">
-        <v>111</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
         <v>113</v>
       </c>
-      <c r="X7" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>114</v>
       </c>
-      <c r="AA7" t="s">
-        <v>115</v>
-      </c>
       <c r="AB7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AC7" t="b">
         <v>0</v>
       </c>
       <c r="AD7" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7" t="s">
         <v>137</v>
       </c>
-      <c r="AE7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF7">
-        <v>0</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>138</v>
       </c>
-      <c r="AH7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI7">
-        <v>0</v>
-      </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>139</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="s">
         <v>140</v>
       </c>
-      <c r="AL7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="s">
         <v>141</v>
       </c>
-      <c r="AO7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP7">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>142</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>143</v>
       </c>
-      <c r="AS7" t="s">
-        <v>144</v>
-      </c>
       <c r="AT7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU7" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV7" t="s">
         <v>148</v>
       </c>
-      <c r="AV7" t="s">
+      <c r="AW7" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX7">
+        <v>0</v>
+      </c>
+      <c r="AY7" t="s">
         <v>149</v>
       </c>
-      <c r="AW7" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX7">
-        <v>0</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:53">
@@ -1999,136 +1996,136 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K8" t="s">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s">
         <v>105</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
+        <v>104</v>
+      </c>
+      <c r="N8" t="s">
         <v>106</v>
       </c>
-      <c r="M8" t="s">
-        <v>105</v>
-      </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>107</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>108</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>109</v>
       </c>
-      <c r="Q8" t="s">
-        <v>110</v>
-      </c>
       <c r="R8" t="s">
+        <v>110</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
         <v>111</v>
       </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
+        <v>110</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8" t="s">
         <v>112</v>
       </c>
-      <c r="U8" t="s">
-        <v>111</v>
-      </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8" t="s">
         <v>113</v>
       </c>
-      <c r="X8" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>114</v>
       </c>
-      <c r="AA8" t="s">
-        <v>115</v>
-      </c>
       <c r="AB8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AC8" t="b">
         <v>0</v>
       </c>
       <c r="AD8" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF8">
+        <v>2</v>
+      </c>
+      <c r="AG8" t="s">
         <v>137</v>
       </c>
-      <c r="AE8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF8">
-        <v>2</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI8">
+        <v>2</v>
+      </c>
+      <c r="AJ8" t="s">
         <v>138</v>
       </c>
-      <c r="AH8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI8">
-        <v>2</v>
-      </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>139</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AL8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM8">
+        <v>2</v>
+      </c>
+      <c r="AN8" t="s">
         <v>140</v>
       </c>
-      <c r="AL8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM8">
-        <v>2</v>
-      </c>
-      <c r="AN8" t="s">
+      <c r="AO8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>141</v>
       </c>
-      <c r="AO8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-      <c r="AQ8" t="s">
+      <c r="AR8" t="s">
         <v>142</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AS8" t="s">
         <v>143</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="AT8" t="s">
         <v>144</v>
       </c>
-      <c r="AT8" t="s">
-        <v>145</v>
-      </c>
       <c r="AU8" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV8" t="s">
         <v>148</v>
       </c>
-      <c r="AV8" t="s">
+      <c r="AW8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX8">
+        <v>0</v>
+      </c>
+      <c r="AY8" t="s">
         <v>149</v>
       </c>
-      <c r="AW8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX8">
-        <v>0</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:53">
@@ -2151,136 +2148,136 @@
         <v>0</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K9" t="s">
+        <v>104</v>
+      </c>
+      <c r="L9" t="s">
         <v>105</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>104</v>
+      </c>
+      <c r="N9" t="s">
         <v>106</v>
       </c>
-      <c r="M9" t="s">
-        <v>105</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>107</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>108</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>109</v>
       </c>
-      <c r="Q9" t="s">
-        <v>110</v>
-      </c>
       <c r="R9" t="s">
+        <v>110</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
         <v>111</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
+        <v>110</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9" t="s">
         <v>112</v>
       </c>
-      <c r="U9" t="s">
-        <v>111</v>
-      </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
         <v>113</v>
       </c>
-      <c r="X9" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>114</v>
       </c>
-      <c r="AA9" t="s">
-        <v>115</v>
-      </c>
       <c r="AB9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC9" t="b">
         <v>0</v>
       </c>
       <c r="AD9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF9">
+        <v>2</v>
+      </c>
+      <c r="AG9" t="s">
         <v>137</v>
       </c>
-      <c r="AE9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF9">
-        <v>2</v>
-      </c>
-      <c r="AG9" t="s">
+      <c r="AH9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI9">
+        <v>2</v>
+      </c>
+      <c r="AJ9" t="s">
         <v>138</v>
       </c>
-      <c r="AH9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI9">
-        <v>2</v>
-      </c>
-      <c r="AJ9" t="s">
+      <c r="AK9" t="s">
         <v>139</v>
       </c>
-      <c r="AK9" t="s">
+      <c r="AL9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM9">
+        <v>2</v>
+      </c>
+      <c r="AN9" t="s">
         <v>140</v>
       </c>
-      <c r="AL9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM9">
-        <v>2</v>
-      </c>
-      <c r="AN9" t="s">
+      <c r="AO9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9" t="s">
         <v>141</v>
       </c>
-      <c r="AO9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP9">
-        <v>0</v>
-      </c>
-      <c r="AQ9" t="s">
+      <c r="AR9" t="s">
         <v>142</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AS9" t="s">
         <v>143</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AT9" t="s">
         <v>144</v>
       </c>
-      <c r="AT9" t="s">
-        <v>145</v>
-      </c>
       <c r="AU9" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV9" t="s">
         <v>148</v>
       </c>
-      <c r="AV9" t="s">
+      <c r="AW9" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX9">
+        <v>0</v>
+      </c>
+      <c r="AY9" t="s">
         <v>149</v>
       </c>
-      <c r="AW9" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX9">
-        <v>0</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:53">
@@ -2303,136 +2300,136 @@
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K10" t="s">
+        <v>104</v>
+      </c>
+      <c r="L10" t="s">
         <v>105</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N10" t="s">
         <v>106</v>
       </c>
-      <c r="M10" t="s">
-        <v>105</v>
-      </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>107</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>108</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>109</v>
       </c>
-      <c r="Q10" t="s">
-        <v>110</v>
-      </c>
       <c r="R10" t="s">
+        <v>110</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10" t="s">
         <v>111</v>
       </c>
-      <c r="S10">
-        <v>2</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
+        <v>110</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10" t="s">
         <v>112</v>
       </c>
-      <c r="U10" t="s">
-        <v>111</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10" t="s">
         <v>113</v>
       </c>
-      <c r="X10" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>114</v>
       </c>
-      <c r="AA10" t="s">
-        <v>115</v>
-      </c>
       <c r="AB10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC10" t="b">
         <v>0</v>
       </c>
       <c r="AD10" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF10">
+        <v>2</v>
+      </c>
+      <c r="AG10" t="s">
         <v>137</v>
       </c>
-      <c r="AE10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF10">
-        <v>2</v>
-      </c>
-      <c r="AG10" t="s">
+      <c r="AH10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="s">
         <v>138</v>
       </c>
-      <c r="AH10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
-      </c>
-      <c r="AJ10" t="s">
+      <c r="AK10" t="s">
         <v>139</v>
       </c>
-      <c r="AK10" t="s">
+      <c r="AL10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM10">
+        <v>2</v>
+      </c>
+      <c r="AN10" t="s">
         <v>140</v>
       </c>
-      <c r="AL10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM10">
-        <v>2</v>
-      </c>
-      <c r="AN10" t="s">
+      <c r="AO10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10" t="s">
         <v>141</v>
       </c>
-      <c r="AO10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-      <c r="AQ10" t="s">
+      <c r="AR10" t="s">
         <v>142</v>
       </c>
-      <c r="AR10" t="s">
+      <c r="AS10" t="s">
         <v>143</v>
       </c>
-      <c r="AS10" t="s">
-        <v>144</v>
-      </c>
       <c r="AT10" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU10" t="s">
         <v>147</v>
       </c>
-      <c r="AU10" t="s">
+      <c r="AV10" t="s">
         <v>148</v>
       </c>
-      <c r="AV10" t="s">
+      <c r="AW10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10" t="s">
         <v>149</v>
       </c>
-      <c r="AW10" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX10">
-        <v>0</v>
-      </c>
-      <c r="AY10" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:53">
@@ -2455,136 +2452,136 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K11" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" t="s">
         <v>105</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11" t="s">
         <v>106</v>
       </c>
-      <c r="M11" t="s">
-        <v>105</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>107</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>108</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>109</v>
       </c>
-      <c r="Q11" t="s">
-        <v>110</v>
-      </c>
       <c r="R11" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
         <v>111</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11" t="s">
+      <c r="U11" t="s">
+        <v>110</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11" t="s">
         <v>112</v>
       </c>
-      <c r="U11" t="s">
-        <v>111</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
         <v>113</v>
       </c>
-      <c r="X11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>114</v>
       </c>
-      <c r="AA11" t="s">
-        <v>115</v>
-      </c>
       <c r="AB11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AC11" t="b">
         <v>0</v>
       </c>
       <c r="AD11" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF11">
+        <v>2</v>
+      </c>
+      <c r="AG11" t="s">
         <v>137</v>
       </c>
-      <c r="AE11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF11">
-        <v>2</v>
-      </c>
-      <c r="AG11" t="s">
+      <c r="AH11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI11">
+        <v>2</v>
+      </c>
+      <c r="AJ11" t="s">
         <v>138</v>
       </c>
-      <c r="AH11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI11">
-        <v>2</v>
-      </c>
-      <c r="AJ11" t="s">
+      <c r="AK11" t="s">
         <v>139</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AL11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM11">
+        <v>2</v>
+      </c>
+      <c r="AN11" t="s">
         <v>140</v>
       </c>
-      <c r="AL11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM11">
-        <v>2</v>
-      </c>
-      <c r="AN11" t="s">
+      <c r="AO11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11" t="s">
         <v>141</v>
       </c>
-      <c r="AO11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11" t="s">
+      <c r="AR11" t="s">
         <v>142</v>
       </c>
-      <c r="AR11" t="s">
+      <c r="AS11" t="s">
         <v>143</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AT11" t="s">
         <v>144</v>
       </c>
-      <c r="AT11" t="s">
-        <v>145</v>
-      </c>
       <c r="AU11" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV11" t="s">
         <v>148</v>
       </c>
-      <c r="AV11" t="s">
+      <c r="AW11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX11">
+        <v>0</v>
+      </c>
+      <c r="AY11" t="s">
         <v>149</v>
       </c>
-      <c r="AW11" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX11">
-        <v>0</v>
-      </c>
-      <c r="AY11" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:53">
@@ -2607,136 +2604,136 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K12" t="s">
+        <v>104</v>
+      </c>
+      <c r="L12" t="s">
         <v>105</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+      <c r="N12" t="s">
         <v>106</v>
       </c>
-      <c r="M12" t="s">
-        <v>105</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>107</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>108</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>109</v>
       </c>
-      <c r="Q12" t="s">
-        <v>110</v>
-      </c>
       <c r="R12" t="s">
+        <v>110</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
         <v>111</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
+        <v>110</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
         <v>112</v>
       </c>
-      <c r="U12" t="s">
-        <v>111</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
         <v>113</v>
       </c>
-      <c r="X12" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="s">
+      <c r="AA12" t="s">
         <v>114</v>
       </c>
-      <c r="AA12" t="s">
-        <v>115</v>
-      </c>
       <c r="AB12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC12" t="b">
         <v>0</v>
       </c>
       <c r="AD12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12" t="s">
         <v>137</v>
       </c>
-      <c r="AE12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="s">
         <v>138</v>
       </c>
-      <c r="AH12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI12">
-        <v>0</v>
-      </c>
-      <c r="AJ12" t="s">
+      <c r="AK12" t="s">
         <v>139</v>
       </c>
-      <c r="AK12" t="s">
+      <c r="AL12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="s">
         <v>140</v>
       </c>
-      <c r="AL12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM12">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="s">
+      <c r="AO12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP12">
+        <v>0</v>
+      </c>
+      <c r="AQ12" t="s">
         <v>141</v>
       </c>
-      <c r="AO12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
-      <c r="AQ12" t="s">
+      <c r="AR12" t="s">
         <v>142</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AS12" t="s">
         <v>143</v>
       </c>
-      <c r="AS12" t="s">
-        <v>144</v>
-      </c>
       <c r="AT12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU12" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV12" t="s">
         <v>148</v>
       </c>
-      <c r="AV12" t="s">
+      <c r="AW12" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12" t="s">
         <v>149</v>
       </c>
-      <c r="AW12" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:53">
@@ -2759,136 +2756,136 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L13" t="s">
         <v>105</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
+        <v>104</v>
+      </c>
+      <c r="N13" t="s">
         <v>106</v>
       </c>
-      <c r="M13" t="s">
-        <v>105</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>107</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>108</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>109</v>
       </c>
-      <c r="Q13" t="s">
-        <v>110</v>
-      </c>
       <c r="R13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="S13">
         <v>1</v>
       </c>
       <c r="T13" t="s">
+        <v>111</v>
+      </c>
+      <c r="U13" t="s">
+        <v>110</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
         <v>112</v>
       </c>
-      <c r="U13" t="s">
-        <v>111</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13" t="s">
+      <c r="X13" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
         <v>113</v>
       </c>
-      <c r="X13" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13" t="s">
+      <c r="AA13" t="s">
         <v>114</v>
       </c>
-      <c r="AA13" t="s">
-        <v>115</v>
-      </c>
       <c r="AB13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AC13" t="b">
         <v>0</v>
       </c>
       <c r="AD13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AE13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AF13">
         <v>3</v>
       </c>
       <c r="AG13" t="s">
+        <v>137</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI13">
+        <v>2</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>138</v>
       </c>
-      <c r="AH13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI13">
-        <v>2</v>
-      </c>
-      <c r="AJ13" t="s">
+      <c r="AK13" t="s">
         <v>139</v>
       </c>
-      <c r="AK13" t="s">
-        <v>140</v>
-      </c>
       <c r="AL13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM13">
         <v>3</v>
       </c>
       <c r="AN13" t="s">
+        <v>140</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP13">
+        <v>0</v>
+      </c>
+      <c r="AQ13" t="s">
         <v>141</v>
       </c>
-      <c r="AO13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP13">
-        <v>0</v>
-      </c>
-      <c r="AQ13" t="s">
+      <c r="AR13" t="s">
         <v>142</v>
       </c>
-      <c r="AR13" t="s">
+      <c r="AS13" t="s">
         <v>143</v>
       </c>
-      <c r="AS13" t="s">
+      <c r="AT13" t="s">
         <v>144</v>
       </c>
-      <c r="AT13" t="s">
-        <v>145</v>
-      </c>
       <c r="AU13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV13" t="s">
         <v>148</v>
       </c>
-      <c r="AV13" t="s">
+      <c r="AW13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX13">
+        <v>0</v>
+      </c>
+      <c r="AY13" t="s">
         <v>149</v>
       </c>
-      <c r="AW13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX13">
-        <v>0</v>
-      </c>
-      <c r="AY13" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:53">
@@ -2911,136 +2908,136 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" t="s">
         <v>105</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
+        <v>104</v>
+      </c>
+      <c r="N14" t="s">
         <v>106</v>
       </c>
-      <c r="M14" t="s">
-        <v>105</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>107</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>108</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>109</v>
       </c>
-      <c r="Q14" t="s">
-        <v>110</v>
-      </c>
       <c r="R14" t="s">
+        <v>110</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
         <v>111</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
+        <v>110</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14" t="s">
         <v>112</v>
       </c>
-      <c r="U14" t="s">
-        <v>111</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
         <v>113</v>
       </c>
-      <c r="X14" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="s">
+      <c r="AA14" t="s">
         <v>114</v>
       </c>
-      <c r="AA14" t="s">
-        <v>115</v>
-      </c>
       <c r="AB14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AC14" t="b">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF14">
+        <v>2</v>
+      </c>
+      <c r="AG14" t="s">
         <v>137</v>
       </c>
-      <c r="AE14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF14">
-        <v>2</v>
-      </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI14">
+        <v>2</v>
+      </c>
+      <c r="AJ14" t="s">
         <v>138</v>
       </c>
-      <c r="AH14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI14">
-        <v>2</v>
-      </c>
-      <c r="AJ14" t="s">
+      <c r="AK14" t="s">
         <v>139</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AL14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM14">
+        <v>2</v>
+      </c>
+      <c r="AN14" t="s">
         <v>140</v>
       </c>
-      <c r="AL14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM14">
-        <v>2</v>
-      </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP14">
+        <v>0</v>
+      </c>
+      <c r="AQ14" t="s">
         <v>141</v>
       </c>
-      <c r="AO14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP14">
-        <v>0</v>
-      </c>
-      <c r="AQ14" t="s">
+      <c r="AR14" t="s">
         <v>142</v>
       </c>
-      <c r="AR14" t="s">
+      <c r="AS14" t="s">
         <v>143</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AT14" t="s">
         <v>144</v>
       </c>
-      <c r="AT14" t="s">
-        <v>145</v>
-      </c>
       <c r="AU14" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV14" t="s">
         <v>148</v>
       </c>
-      <c r="AV14" t="s">
+      <c r="AW14" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX14">
+        <v>0</v>
+      </c>
+      <c r="AY14" t="s">
         <v>149</v>
       </c>
-      <c r="AW14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX14">
-        <v>0</v>
-      </c>
-      <c r="AY14" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:53">
@@ -3063,136 +3060,136 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K15" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" t="s">
         <v>105</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
+        <v>104</v>
+      </c>
+      <c r="N15" t="s">
         <v>106</v>
       </c>
-      <c r="M15" t="s">
-        <v>105</v>
-      </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>107</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>108</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>109</v>
       </c>
-      <c r="Q15" t="s">
-        <v>110</v>
-      </c>
       <c r="R15" t="s">
+        <v>110</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
         <v>111</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
+        <v>110</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
         <v>112</v>
       </c>
-      <c r="U15" t="s">
-        <v>111</v>
-      </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15" t="s">
+      <c r="X15" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
         <v>113</v>
       </c>
-      <c r="X15" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
+      <c r="AA15" t="s">
         <v>114</v>
       </c>
-      <c r="AA15" t="s">
-        <v>115</v>
-      </c>
       <c r="AB15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC15" t="b">
         <v>0</v>
       </c>
       <c r="AD15" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15" t="s">
         <v>137</v>
       </c>
-      <c r="AE15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-      <c r="AG15" t="s">
+      <c r="AH15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="s">
         <v>138</v>
       </c>
-      <c r="AH15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI15">
-        <v>0</v>
-      </c>
-      <c r="AJ15" t="s">
+      <c r="AK15" t="s">
         <v>139</v>
       </c>
-      <c r="AK15" t="s">
+      <c r="AL15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15" t="s">
         <v>140</v>
       </c>
-      <c r="AL15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM15">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15" t="s">
         <v>141</v>
       </c>
-      <c r="AO15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-      <c r="AQ15" t="s">
+      <c r="AR15" t="s">
         <v>142</v>
       </c>
-      <c r="AR15" t="s">
+      <c r="AS15" t="s">
         <v>143</v>
       </c>
-      <c r="AS15" t="s">
-        <v>144</v>
-      </c>
       <c r="AT15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU15" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV15" t="s">
         <v>148</v>
       </c>
-      <c r="AV15" t="s">
+      <c r="AW15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX15">
+        <v>0</v>
+      </c>
+      <c r="AY15" t="s">
         <v>149</v>
       </c>
-      <c r="AW15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX15">
-        <v>0</v>
-      </c>
-      <c r="AY15" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:53">
@@ -3206,7 +3203,7 @@
         <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" t="b">
         <v>0</v>
@@ -3215,136 +3212,136 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K16" t="s">
+        <v>104</v>
+      </c>
+      <c r="L16" t="s">
         <v>105</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
+        <v>104</v>
+      </c>
+      <c r="N16" t="s">
         <v>106</v>
       </c>
-      <c r="M16" t="s">
-        <v>105</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>107</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>108</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>109</v>
       </c>
-      <c r="Q16" t="s">
-        <v>110</v>
-      </c>
       <c r="R16" t="s">
+        <v>110</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="T16" t="s">
         <v>111</v>
       </c>
-      <c r="S16">
-        <v>2</v>
-      </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
+        <v>110</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
         <v>112</v>
       </c>
-      <c r="U16" t="s">
-        <v>111</v>
-      </c>
-      <c r="V16">
-        <v>0</v>
-      </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
         <v>113</v>
       </c>
-      <c r="X16" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="s">
+      <c r="AA16" t="s">
         <v>114</v>
       </c>
-      <c r="AA16" t="s">
-        <v>115</v>
-      </c>
       <c r="AB16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AC16" t="b">
         <v>0</v>
       </c>
       <c r="AD16" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF16">
+        <v>2</v>
+      </c>
+      <c r="AG16" t="s">
         <v>137</v>
       </c>
-      <c r="AE16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF16">
-        <v>2</v>
-      </c>
-      <c r="AG16" t="s">
+      <c r="AH16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16" t="s">
         <v>138</v>
       </c>
-      <c r="AH16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI16">
-        <v>0</v>
-      </c>
-      <c r="AJ16" t="s">
+      <c r="AK16" t="s">
         <v>139</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AL16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM16">
+        <v>2</v>
+      </c>
+      <c r="AN16" t="s">
         <v>140</v>
       </c>
-      <c r="AL16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM16">
-        <v>2</v>
-      </c>
-      <c r="AN16" t="s">
+      <c r="AO16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16" t="s">
         <v>141</v>
       </c>
-      <c r="AO16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP16">
-        <v>0</v>
-      </c>
-      <c r="AQ16" t="s">
+      <c r="AR16" t="s">
         <v>142</v>
       </c>
-      <c r="AR16" t="s">
+      <c r="AS16" t="s">
         <v>143</v>
       </c>
-      <c r="AS16" t="s">
-        <v>144</v>
-      </c>
       <c r="AT16" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU16" t="s">
         <v>147</v>
       </c>
-      <c r="AU16" t="s">
+      <c r="AV16" t="s">
         <v>148</v>
       </c>
-      <c r="AV16" t="s">
+      <c r="AW16" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX16">
+        <v>0</v>
+      </c>
+      <c r="AY16" t="s">
         <v>149</v>
       </c>
-      <c r="AW16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX16">
-        <v>0</v>
-      </c>
-      <c r="AY16" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:53">
@@ -3358,7 +3355,7 @@
         <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -3367,136 +3364,136 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K17" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" t="s">
         <v>105</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
+        <v>104</v>
+      </c>
+      <c r="N17" t="s">
         <v>106</v>
       </c>
-      <c r="M17" t="s">
-        <v>105</v>
-      </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>107</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>108</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>109</v>
       </c>
-      <c r="Q17" t="s">
-        <v>110</v>
-      </c>
       <c r="R17" t="s">
+        <v>110</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
         <v>111</v>
       </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
+        <v>110</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17" t="s">
         <v>112</v>
       </c>
-      <c r="U17" t="s">
-        <v>111</v>
-      </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
         <v>113</v>
       </c>
-      <c r="X17" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="AA17" t="s">
         <v>114</v>
       </c>
-      <c r="AA17" t="s">
-        <v>115</v>
-      </c>
       <c r="AB17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AC17" t="b">
         <v>0</v>
       </c>
       <c r="AD17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17" t="s">
         <v>137</v>
       </c>
-      <c r="AE17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF17">
-        <v>0</v>
-      </c>
-      <c r="AG17" t="s">
+      <c r="AH17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17" t="s">
         <v>138</v>
       </c>
-      <c r="AH17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI17">
-        <v>0</v>
-      </c>
-      <c r="AJ17" t="s">
+      <c r="AK17" t="s">
         <v>139</v>
       </c>
-      <c r="AK17" t="s">
+      <c r="AL17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17" t="s">
         <v>140</v>
       </c>
-      <c r="AL17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM17">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="s">
+      <c r="AO17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17" t="s">
         <v>141</v>
       </c>
-      <c r="AO17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP17">
-        <v>0</v>
-      </c>
-      <c r="AQ17" t="s">
+      <c r="AR17" t="s">
         <v>142</v>
       </c>
-      <c r="AR17" t="s">
+      <c r="AS17" t="s">
         <v>143</v>
       </c>
-      <c r="AS17" t="s">
-        <v>144</v>
-      </c>
       <c r="AT17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AU17" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV17" t="s">
         <v>148</v>
       </c>
-      <c r="AV17" t="s">
+      <c r="AW17" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX17">
+        <v>0</v>
+      </c>
+      <c r="AY17" t="s">
         <v>149</v>
       </c>
-      <c r="AW17" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX17">
-        <v>0</v>
-      </c>
-      <c r="AY17" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:53">
@@ -3510,7 +3507,7 @@
         <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -3519,136 +3516,136 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K18" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" t="s">
         <v>105</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
+        <v>104</v>
+      </c>
+      <c r="N18" t="s">
         <v>106</v>
       </c>
-      <c r="M18" t="s">
-        <v>105</v>
-      </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>107</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>108</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>109</v>
       </c>
-      <c r="Q18" t="s">
-        <v>110</v>
-      </c>
       <c r="R18" t="s">
+        <v>110</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
         <v>111</v>
       </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>112</v>
-      </c>
       <c r="U18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V18">
         <v>1</v>
       </c>
       <c r="W18" t="s">
+        <v>112</v>
+      </c>
+      <c r="X18" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
         <v>113</v>
       </c>
-      <c r="X18" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="s">
+      <c r="AA18" t="s">
         <v>114</v>
       </c>
-      <c r="AA18" t="s">
-        <v>115</v>
-      </c>
       <c r="AB18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC18" t="b">
         <v>0</v>
       </c>
       <c r="AD18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18" t="s">
         <v>137</v>
       </c>
-      <c r="AE18" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF18">
-        <v>0</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>138</v>
-      </c>
       <c r="AH18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AI18">
         <v>1.5</v>
       </c>
       <c r="AJ18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AK18" t="s">
         <v>139</v>
       </c>
-      <c r="AK18" t="s">
-        <v>140</v>
-      </c>
       <c r="AL18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AM18">
         <v>1.5</v>
       </c>
       <c r="AN18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AO18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AP18">
         <v>1</v>
       </c>
       <c r="AQ18" t="s">
+        <v>141</v>
+      </c>
+      <c r="AR18" t="s">
         <v>142</v>
       </c>
-      <c r="AR18" t="s">
+      <c r="AS18" t="s">
         <v>143</v>
       </c>
-      <c r="AS18" t="s">
+      <c r="AT18" t="s">
         <v>144</v>
       </c>
-      <c r="AT18" t="s">
-        <v>145</v>
-      </c>
       <c r="AU18" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV18" t="s">
         <v>148</v>
       </c>
-      <c r="AV18" t="s">
+      <c r="AW18" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX18">
+        <v>0</v>
+      </c>
+      <c r="AY18" t="s">
         <v>149</v>
       </c>
-      <c r="AW18" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX18">
-        <v>0</v>
-      </c>
-      <c r="AY18" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:53">
@@ -3662,7 +3659,7 @@
         <v>81</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -3671,136 +3668,136 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K19" t="s">
+        <v>104</v>
+      </c>
+      <c r="L19" t="s">
         <v>105</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
+        <v>104</v>
+      </c>
+      <c r="N19" t="s">
         <v>106</v>
       </c>
-      <c r="M19" t="s">
-        <v>105</v>
-      </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>107</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>108</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>109</v>
       </c>
-      <c r="Q19" t="s">
-        <v>110</v>
-      </c>
       <c r="R19" t="s">
+        <v>110</v>
+      </c>
+      <c r="S19">
+        <v>2</v>
+      </c>
+      <c r="T19" t="s">
         <v>111</v>
       </c>
-      <c r="S19">
-        <v>2</v>
-      </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
+        <v>110</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
         <v>112</v>
       </c>
-      <c r="U19" t="s">
-        <v>111</v>
-      </c>
-      <c r="V19">
-        <v>0</v>
-      </c>
-      <c r="W19" t="s">
+      <c r="X19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
         <v>113</v>
       </c>
-      <c r="X19" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
+      <c r="AA19" t="s">
         <v>114</v>
       </c>
-      <c r="AA19" t="s">
-        <v>115</v>
-      </c>
       <c r="AB19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AC19" t="b">
         <v>0</v>
       </c>
       <c r="AD19" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF19">
+        <v>2</v>
+      </c>
+      <c r="AG19" t="s">
         <v>137</v>
       </c>
-      <c r="AE19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF19">
-        <v>2</v>
-      </c>
-      <c r="AG19" t="s">
+      <c r="AH19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19" t="s">
         <v>138</v>
       </c>
-      <c r="AH19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI19">
-        <v>0</v>
-      </c>
-      <c r="AJ19" t="s">
+      <c r="AK19" t="s">
         <v>139</v>
       </c>
-      <c r="AK19" t="s">
+      <c r="AL19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM19">
+        <v>2</v>
+      </c>
+      <c r="AN19" t="s">
         <v>140</v>
       </c>
-      <c r="AL19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM19">
-        <v>2</v>
-      </c>
-      <c r="AN19" t="s">
+      <c r="AO19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19" t="s">
         <v>141</v>
       </c>
-      <c r="AO19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP19">
-        <v>0</v>
-      </c>
-      <c r="AQ19" t="s">
+      <c r="AR19" t="s">
         <v>142</v>
       </c>
-      <c r="AR19" t="s">
+      <c r="AS19" t="s">
         <v>143</v>
       </c>
-      <c r="AS19" t="s">
-        <v>144</v>
-      </c>
       <c r="AT19" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU19" t="s">
         <v>147</v>
       </c>
-      <c r="AU19" t="s">
+      <c r="AV19" t="s">
         <v>148</v>
       </c>
-      <c r="AV19" t="s">
+      <c r="AW19" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX19">
+        <v>0</v>
+      </c>
+      <c r="AY19" t="s">
         <v>149</v>
       </c>
-      <c r="AW19" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX19">
-        <v>0</v>
-      </c>
-      <c r="AY19" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:53">
@@ -3814,7 +3811,7 @@
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -3823,136 +3820,136 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K20" t="s">
+        <v>104</v>
+      </c>
+      <c r="L20" t="s">
         <v>105</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
+        <v>104</v>
+      </c>
+      <c r="N20" t="s">
         <v>106</v>
       </c>
-      <c r="M20" t="s">
-        <v>105</v>
-      </c>
-      <c r="N20" t="s">
+      <c r="O20" t="s">
         <v>107</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>108</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>109</v>
       </c>
-      <c r="Q20" t="s">
-        <v>110</v>
-      </c>
       <c r="R20" t="s">
+        <v>110</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
         <v>111</v>
       </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
+        <v>110</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20" t="s">
         <v>112</v>
       </c>
-      <c r="U20" t="s">
-        <v>111</v>
-      </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="X20" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
         <v>113</v>
       </c>
-      <c r="X20" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="Z20" t="s">
+      <c r="AA20" t="s">
         <v>114</v>
       </c>
-      <c r="AA20" t="s">
-        <v>115</v>
-      </c>
       <c r="AB20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC20" t="b">
         <v>0</v>
       </c>
       <c r="AD20" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF20">
+        <v>2</v>
+      </c>
+      <c r="AG20" t="s">
         <v>137</v>
       </c>
-      <c r="AE20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF20">
-        <v>2</v>
-      </c>
-      <c r="AG20" t="s">
+      <c r="AH20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI20">
+        <v>2</v>
+      </c>
+      <c r="AJ20" t="s">
         <v>138</v>
       </c>
-      <c r="AH20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI20">
-        <v>2</v>
-      </c>
-      <c r="AJ20" t="s">
+      <c r="AK20" t="s">
         <v>139</v>
       </c>
-      <c r="AK20" t="s">
+      <c r="AL20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM20">
+        <v>2</v>
+      </c>
+      <c r="AN20" t="s">
         <v>140</v>
       </c>
-      <c r="AL20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM20">
-        <v>2</v>
-      </c>
-      <c r="AN20" t="s">
+      <c r="AO20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20" t="s">
         <v>141</v>
       </c>
-      <c r="AO20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP20">
-        <v>0</v>
-      </c>
-      <c r="AQ20" t="s">
+      <c r="AR20" t="s">
         <v>142</v>
       </c>
-      <c r="AR20" t="s">
+      <c r="AS20" t="s">
         <v>143</v>
       </c>
-      <c r="AS20" t="s">
+      <c r="AT20" t="s">
         <v>144</v>
       </c>
-      <c r="AT20" t="s">
-        <v>145</v>
-      </c>
       <c r="AU20" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV20" t="s">
         <v>148</v>
       </c>
-      <c r="AV20" t="s">
+      <c r="AW20" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX20">
+        <v>0</v>
+      </c>
+      <c r="AY20" t="s">
         <v>149</v>
       </c>
-      <c r="AW20" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX20">
-        <v>0</v>
-      </c>
-      <c r="AY20" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:53">
@@ -3966,7 +3963,7 @@
         <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -3975,136 +3972,136 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" t="s">
         <v>105</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
+        <v>104</v>
+      </c>
+      <c r="N21" t="s">
         <v>106</v>
       </c>
-      <c r="M21" t="s">
-        <v>105</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="O21" t="s">
         <v>107</v>
       </c>
-      <c r="O21" t="s">
+      <c r="P21" t="s">
         <v>108</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>109</v>
       </c>
-      <c r="Q21" t="s">
-        <v>110</v>
-      </c>
       <c r="R21" t="s">
+        <v>110</v>
+      </c>
+      <c r="S21">
+        <v>2</v>
+      </c>
+      <c r="T21" t="s">
         <v>111</v>
       </c>
-      <c r="S21">
-        <v>2</v>
-      </c>
-      <c r="T21" t="s">
+      <c r="U21" t="s">
+        <v>110</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21" t="s">
         <v>112</v>
       </c>
-      <c r="U21" t="s">
-        <v>111</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21" t="s">
+      <c r="X21" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
         <v>113</v>
       </c>
-      <c r="X21" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="s">
+      <c r="AA21" t="s">
         <v>114</v>
       </c>
-      <c r="AA21" t="s">
-        <v>115</v>
-      </c>
       <c r="AB21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AC21" t="b">
         <v>0</v>
       </c>
       <c r="AD21" t="s">
+        <v>136</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF21">
+        <v>2</v>
+      </c>
+      <c r="AG21" t="s">
         <v>137</v>
       </c>
-      <c r="AE21" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF21">
-        <v>2</v>
-      </c>
-      <c r="AG21" t="s">
+      <c r="AH21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21" t="s">
         <v>138</v>
       </c>
-      <c r="AH21" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI21">
-        <v>0</v>
-      </c>
-      <c r="AJ21" t="s">
+      <c r="AK21" t="s">
         <v>139</v>
       </c>
-      <c r="AK21" t="s">
+      <c r="AL21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM21">
+        <v>2</v>
+      </c>
+      <c r="AN21" t="s">
         <v>140</v>
       </c>
-      <c r="AL21" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM21">
-        <v>2</v>
-      </c>
-      <c r="AN21" t="s">
+      <c r="AO21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP21">
+        <v>0</v>
+      </c>
+      <c r="AQ21" t="s">
         <v>141</v>
       </c>
-      <c r="AO21" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-      <c r="AQ21" t="s">
+      <c r="AR21" t="s">
         <v>142</v>
       </c>
-      <c r="AR21" t="s">
+      <c r="AS21" t="s">
         <v>143</v>
       </c>
-      <c r="AS21" t="s">
-        <v>144</v>
-      </c>
       <c r="AT21" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU21" t="s">
         <v>147</v>
       </c>
-      <c r="AU21" t="s">
+      <c r="AV21" t="s">
         <v>148</v>
       </c>
-      <c r="AV21" t="s">
+      <c r="AW21" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX21">
+        <v>0</v>
+      </c>
+      <c r="AY21" t="s">
         <v>149</v>
       </c>
-      <c r="AW21" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX21">
-        <v>0</v>
-      </c>
-      <c r="AY21" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:53">
@@ -4118,7 +4115,7 @@
         <v>81</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -4127,136 +4124,136 @@
         <v>0</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K22" t="s">
         <v>104</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>105</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" t="s">
         <v>106</v>
       </c>
-      <c r="M22" t="s">
-        <v>105</v>
-      </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>107</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>108</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>109</v>
       </c>
-      <c r="Q22" t="s">
-        <v>110</v>
-      </c>
       <c r="R22" t="s">
+        <v>110</v>
+      </c>
+      <c r="S22">
+        <v>2</v>
+      </c>
+      <c r="T22" t="s">
         <v>111</v>
       </c>
-      <c r="S22">
-        <v>2</v>
-      </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
+        <v>110</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22" t="s">
         <v>112</v>
       </c>
-      <c r="U22" t="s">
-        <v>111</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
         <v>113</v>
       </c>
-      <c r="X22" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>114</v>
       </c>
-      <c r="AA22" t="s">
-        <v>115</v>
-      </c>
       <c r="AB22" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD22" t="s">
         <v>136</v>
       </c>
-      <c r="AC22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF22">
+        <v>2</v>
+      </c>
+      <c r="AG22" t="s">
         <v>137</v>
       </c>
-      <c r="AE22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF22">
-        <v>2</v>
-      </c>
-      <c r="AG22" t="s">
+      <c r="AH22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="s">
         <v>138</v>
       </c>
-      <c r="AH22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI22">
-        <v>0</v>
-      </c>
-      <c r="AJ22" t="s">
+      <c r="AK22" t="s">
         <v>139</v>
       </c>
-      <c r="AK22" t="s">
+      <c r="AL22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AM22">
+        <v>2</v>
+      </c>
+      <c r="AN22" t="s">
         <v>140</v>
       </c>
-      <c r="AL22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM22">
-        <v>2</v>
-      </c>
-      <c r="AN22" t="s">
+      <c r="AO22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AP22">
+        <v>0</v>
+      </c>
+      <c r="AQ22" t="s">
         <v>141</v>
       </c>
-      <c r="AO22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP22">
-        <v>0</v>
-      </c>
-      <c r="AQ22" t="s">
+      <c r="AR22" t="s">
         <v>142</v>
       </c>
-      <c r="AR22" t="s">
+      <c r="AS22" t="s">
         <v>143</v>
       </c>
-      <c r="AS22" t="s">
-        <v>144</v>
-      </c>
       <c r="AT22" t="s">
+        <v>146</v>
+      </c>
+      <c r="AU22" t="s">
         <v>147</v>
       </c>
-      <c r="AU22" t="s">
+      <c r="AV22" t="s">
         <v>148</v>
       </c>
-      <c r="AV22" t="s">
+      <c r="AW22" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX22">
+        <v>0</v>
+      </c>
+      <c r="AY22" t="s">
         <v>149</v>
       </c>
-      <c r="AW22" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX22">
-        <v>0</v>
-      </c>
-      <c r="AY22" t="s">
-        <v>150</v>
-      </c>
       <c r="AZ22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BA22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>